<commit_message>
New words and +2Lvl`s
</commit_message>
<xml_diff>
--- a/Assets/EntryWords.xlsx
+++ b/Assets/EntryWords.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Затягнутість</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>entry.422429688</t>
+  </si>
+  <si>
+    <t>Медіапростір</t>
+  </si>
+  <si>
+    <t>entry.1568295105</t>
+  </si>
+  <si>
+    <t>Місцеперебування</t>
+  </si>
+  <si>
+    <t>entry.283921628</t>
   </si>
 </sst>
 </file>
@@ -396,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +500,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
+3 lvl, words, new parse&changes in main menu
</commit_message>
<xml_diff>
--- a/Assets/EntryWords.xlsx
+++ b/Assets/EntryWords.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Затягнутість</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>entry.283921628</t>
+  </si>
+  <si>
+    <t>Армагедон</t>
+  </si>
+  <si>
+    <t>entry.934056410</t>
+  </si>
+  <si>
+    <t>Електроопора</t>
+  </si>
+  <si>
+    <t>entry.1240912437</t>
+  </si>
+  <si>
+    <t>Комплімент</t>
+  </si>
+  <si>
+    <t>entry.2030694513</t>
   </si>
 </sst>
 </file>
@@ -408,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,6 +534,30 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>